<commit_message>
Added test for an empty column.
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="319" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="203" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="testfixed_converted.csv" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>text</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>empty_column</t>
   </si>
   <si>
     <t>Chicago Reader</t>
@@ -54,12 +57,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
     <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS\ AM/PM" numFmtId="167"/>
-    <numFmt formatCode="MM/DD/YY\ HH:MM\ AM/PM" numFmtId="168"/>
+    <numFmt formatCode="GENERAL" numFmtId="167"/>
+    <numFmt formatCode="HH:MM:SS\ AM/PM" numFmtId="168"/>
+    <numFmt formatCode="MM/DD/YY\ HH:MM\ AM/PM" numFmtId="169"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -130,12 +134,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="168" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="169" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -153,10 +158,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="H2" activeCellId="0" pane="topLeft" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -192,10 +197,13 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>24472</v>
@@ -203,22 +211,23 @@
       <c r="C2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="D2" s="2" t="b">
+      <c r="D2" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.176388888888889</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="5" t="n">
         <v>24472.1763888889</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>16071</v>
@@ -226,22 +235,23 @@
       <c r="C3" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="D3" s="3" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1.27</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>0.62306712962963</v>
       </c>
-      <c r="G3" s="4" t="n">
-        <v>16071.1230671296</v>
+      <c r="G3" s="5" t="n">
+        <v>16071.6230671296</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>5844</v>
@@ -249,22 +259,23 @@
       <c r="C4" s="0" t="n">
         <v>164</v>
       </c>
-      <c r="D4" s="2" t="b">
+      <c r="D4" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>41800000.01</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <v>5844</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xlsx import implemented but broken, due to apparent date-parsing bug in openpyxl?
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr date1904="1" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38240" windowHeight="20840" tabRatio="203"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="20860" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="testfixed_converted.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="130407"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -61,18 +61,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="3">
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Hindi"/>
-      <family val="2"/>
-    </font>
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -102,13 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,17 +439,15 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" style="1"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,18 +483,17 @@
       <c r="C2">
         <v>40</v>
       </c>
-      <c r="D2" s="3" t="b">
-        <f>TRUE()</f>
+      <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.17638888888888901</v>
       </c>
-      <c r="G2" s="5">
-        <v>24472.1763888889</v>
+      <c r="G2" s="4">
+        <v>24472.176388888889</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -511,17 +506,16 @@
       <c r="C3">
         <v>63</v>
       </c>
-      <c r="D3" s="3" t="b">
-        <f>TRUE()</f>
+      <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3">
         <v>1.27</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.62306712962962996</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>16071.6230671296</v>
       </c>
     </row>
@@ -535,17 +529,16 @@
       <c r="C4">
         <v>164</v>
       </c>
-      <c r="D4" s="3" t="b">
-        <f>FALSE()</f>
+      <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4">
         <v>41800000.009999998</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>5844</v>
       </c>
     </row>
@@ -553,11 +546,13 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
examples: add row containing multi-line value
current example xls and xlsx files lack any values containing a line
feed character. I added one
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="4540" yWindow="880" windowWidth="16380" windowHeight="8200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>text</t>
   </si>
@@ -57,6 +61,10 @@
   </si>
   <si>
     <t>Unicode! Σ</t>
+  </si>
+  <si>
+    <t>This row has a
+multi-line value</t>
   </si>
 </sst>
 </file>
@@ -96,13 +104,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,21 +415,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.625"/>
-    <col min="2" max="2" width="11.875" style="1"/>
-    <col min="4" max="4" width="11.125" style="2"/>
-    <col min="6" max="6" width="13.5"/>
-    <col min="7" max="8" width="20.75"/>
-    <col min="9" max="9" width="38.75"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="8.7109375" style="2"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -468,7 +480,7 @@
         <v>24472.1763888889</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -495,7 +507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -519,18 +531,28 @@
         <v>5844</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="26">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mostly functional agate-excel import, but breaking tests.
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>text</t>
   </si>
@@ -30,9 +34,6 @@
   </si>
   <si>
     <t>float</t>
-  </si>
-  <si>
-    <t>time</t>
   </si>
   <si>
     <t>datetime</t>
@@ -63,9 +64,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -96,12 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,21 +403,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.625"/>
-    <col min="2" max="2" width="11.875" style="1"/>
-    <col min="4" max="4" width="11.125" style="2"/>
-    <col min="6" max="6" width="13.5"/>
-    <col min="7" max="8" width="20.75"/>
-    <col min="9" max="9" width="38.75"/>
+    <col min="2" max="2" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,13 +437,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>24472</v>
@@ -462,15 +456,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="4">
-        <v>0.17638888888888901</v>
-      </c>
-      <c r="G2" s="5">
         <v>24472.1763888889</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>16071</v>
@@ -486,18 +477,15 @@
         <v>1.27</v>
       </c>
       <c r="F3" s="4">
-        <v>0.62306712962962996</v>
-      </c>
-      <c r="G3" s="5">
         <v>16071.6230671296</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>5844</v>
@@ -513,24 +501,26 @@
         <v>41800000.009999998</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
         <v>5844</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>